<commit_message>
add some fit model
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\ForGraduate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD918A6-6F84-459F-934E-1D698F533ED6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AF00A5E-93BA-4895-99E4-573C03E519E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1080,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O98"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1156,7 +1156,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C2">
         <v>706</v>
@@ -1167,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="C3">
         <v>738</v>
@@ -1178,7 +1178,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1">
-        <v>0.33</v>
+        <v>0.4</v>
       </c>
       <c r="C4">
         <v>738</v>
@@ -1189,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>0.4</v>
+        <v>0.43</v>
       </c>
       <c r="C5">
         <v>738</v>
@@ -1211,7 +1211,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
         <v>866</v>
@@ -1222,7 +1222,7 @@
         <v>28</v>
       </c>
       <c r="B8" s="1">
-        <v>0.6</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="C8">
         <v>866</v>
@@ -1233,7 +1233,7 @@
         <v>32</v>
       </c>
       <c r="B9" s="1">
-        <v>0.57999999999999996</v>
+        <v>0.6</v>
       </c>
       <c r="C9">
         <v>866</v>
@@ -1287,6 +1287,9 @@
       <c r="A14">
         <v>52</v>
       </c>
+      <c r="B14" s="1">
+        <v>0.7</v>
+      </c>
       <c r="C14">
         <v>873</v>
       </c>
@@ -1394,6 +1397,9 @@
       <c r="A24">
         <v>92</v>
       </c>
+      <c r="B24" s="1">
+        <v>0.84</v>
+      </c>
       <c r="C24">
         <v>1380</v>
       </c>
@@ -1402,6 +1408,9 @@
       <c r="A25">
         <v>96</v>
       </c>
+      <c r="B25" s="1">
+        <v>0.84</v>
+      </c>
       <c r="C25">
         <v>1380</v>
       </c>
@@ -1410,6 +1419,9 @@
       <c r="A26">
         <v>100</v>
       </c>
+      <c r="B26" s="1">
+        <v>0.84</v>
+      </c>
       <c r="C26">
         <v>1380</v>
       </c>
@@ -1418,6 +1430,9 @@
       <c r="A27">
         <v>104</v>
       </c>
+      <c r="B27" s="1">
+        <v>0.84</v>
+      </c>
       <c r="C27">
         <v>1380</v>
       </c>
@@ -1426,6 +1441,9 @@
       <c r="A28">
         <v>108</v>
       </c>
+      <c r="B28" s="1">
+        <v>0.84</v>
+      </c>
       <c r="C28">
         <v>1380</v>
       </c>
@@ -1445,6 +1463,9 @@
       <c r="A30">
         <v>116</v>
       </c>
+      <c r="B30" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C30">
         <v>1380</v>
       </c>
@@ -1453,6 +1474,9 @@
       <c r="A31">
         <v>120</v>
       </c>
+      <c r="B31" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C31">
         <v>1380</v>
       </c>
@@ -1461,6 +1485,9 @@
       <c r="A32">
         <v>124</v>
       </c>
+      <c r="B32" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C32">
         <v>1380</v>
       </c>
@@ -1469,6 +1496,9 @@
       <c r="A33">
         <v>128</v>
       </c>
+      <c r="B33" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C33">
         <v>2404</v>
       </c>
@@ -1477,6 +1507,9 @@
       <c r="A34">
         <v>132</v>
       </c>
+      <c r="B34" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C34">
         <v>2404</v>
       </c>
@@ -1485,6 +1518,9 @@
       <c r="A35">
         <v>136</v>
       </c>
+      <c r="B35" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C35">
         <v>2404</v>
       </c>
@@ -1493,6 +1529,9 @@
       <c r="A36">
         <v>140</v>
       </c>
+      <c r="B36" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C36">
         <v>2404</v>
       </c>
@@ -1501,6 +1540,9 @@
       <c r="A37">
         <v>144</v>
       </c>
+      <c r="B37" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C37">
         <v>2404</v>
       </c>
@@ -1509,6 +1551,9 @@
       <c r="A38">
         <v>148</v>
       </c>
+      <c r="B38" s="1">
+        <v>0.85</v>
+      </c>
       <c r="C38">
         <v>2404</v>
       </c>
@@ -1528,6 +1573,9 @@
       <c r="A40">
         <v>156</v>
       </c>
+      <c r="B40" s="1">
+        <v>0.86</v>
+      </c>
       <c r="C40">
         <v>2404</v>
       </c>
@@ -1536,6 +1584,9 @@
       <c r="A41">
         <v>160</v>
       </c>
+      <c r="B41" s="1">
+        <v>0.87</v>
+      </c>
       <c r="C41">
         <v>2404</v>
       </c>
@@ -1555,6 +1606,9 @@
       <c r="A43">
         <v>168</v>
       </c>
+      <c r="B43" s="1">
+        <v>0.88</v>
+      </c>
       <c r="C43">
         <v>2404</v>
       </c>
@@ -1563,6 +1617,9 @@
       <c r="A44">
         <v>172</v>
       </c>
+      <c r="B44" s="1">
+        <v>0.88</v>
+      </c>
       <c r="C44">
         <v>2404</v>
       </c>
@@ -1571,6 +1628,9 @@
       <c r="A45">
         <v>176</v>
       </c>
+      <c r="B45" s="1">
+        <v>0.89</v>
+      </c>
       <c r="C45">
         <v>2404</v>
       </c>
@@ -1579,6 +1639,9 @@
       <c r="A46">
         <v>180</v>
       </c>
+      <c r="B46" s="1">
+        <v>0.89</v>
+      </c>
       <c r="C46">
         <v>2404</v>
       </c>
@@ -1598,6 +1661,9 @@
       <c r="A48">
         <v>188</v>
       </c>
+      <c r="B48" s="1">
+        <v>0.91</v>
+      </c>
       <c r="C48">
         <v>2404</v>
       </c>
@@ -1606,6 +1672,9 @@
       <c r="A49">
         <v>192</v>
       </c>
+      <c r="B49" s="1">
+        <v>0.92</v>
+      </c>
       <c r="C49">
         <v>2404</v>
       </c>
@@ -1614,6 +1683,9 @@
       <c r="A50">
         <v>196</v>
       </c>
+      <c r="B50" s="1">
+        <v>0.93</v>
+      </c>
       <c r="C50">
         <v>2404</v>
       </c>
@@ -1622,6 +1694,9 @@
       <c r="A51">
         <v>200</v>
       </c>
+      <c r="B51" s="1">
+        <v>0.94</v>
+      </c>
       <c r="C51">
         <v>2404</v>
       </c>
@@ -1630,6 +1705,9 @@
       <c r="A52">
         <v>204</v>
       </c>
+      <c r="B52" s="1">
+        <v>0.94</v>
+      </c>
       <c r="C52">
         <v>2404</v>
       </c>
@@ -1649,6 +1727,9 @@
       <c r="A54">
         <v>212</v>
       </c>
+      <c r="B54" s="1">
+        <v>0.95</v>
+      </c>
       <c r="C54">
         <v>2404</v>
       </c>
@@ -1657,6 +1738,9 @@
       <c r="A55">
         <v>216</v>
       </c>
+      <c r="B55" s="1">
+        <v>0.95</v>
+      </c>
       <c r="C55">
         <v>2404</v>
       </c>
@@ -1665,6 +1749,9 @@
       <c r="A56">
         <v>220</v>
       </c>
+      <c r="B56" s="1">
+        <v>0.95</v>
+      </c>
       <c r="C56">
         <v>2404</v>
       </c>
@@ -1673,6 +1760,9 @@
       <c r="A57">
         <v>224</v>
       </c>
+      <c r="B57" s="1">
+        <v>0.95</v>
+      </c>
       <c r="C57">
         <v>2404</v>
       </c>
@@ -1681,6 +1771,9 @@
       <c r="A58">
         <v>228</v>
       </c>
+      <c r="B58" s="1">
+        <v>0.95</v>
+      </c>
       <c r="C58">
         <v>2404</v>
       </c>
@@ -1700,6 +1793,9 @@
       <c r="A60">
         <v>236</v>
       </c>
+      <c r="B60" s="1">
+        <v>0.96</v>
+      </c>
       <c r="C60">
         <v>2404</v>
       </c>
@@ -1708,6 +1804,9 @@
       <c r="A61">
         <v>240</v>
       </c>
+      <c r="B61" s="1">
+        <v>0.96</v>
+      </c>
       <c r="C61">
         <v>2404</v>
       </c>
@@ -1716,6 +1815,9 @@
       <c r="A62">
         <v>244</v>
       </c>
+      <c r="B62" s="1">
+        <v>0.96</v>
+      </c>
       <c r="C62">
         <v>2404</v>
       </c>
@@ -1724,6 +1826,9 @@
       <c r="A63">
         <v>248</v>
       </c>
+      <c r="B63" s="1">
+        <v>0.96</v>
+      </c>
       <c r="C63">
         <v>2404</v>
       </c>
@@ -1732,6 +1837,9 @@
       <c r="A64">
         <v>252</v>
       </c>
+      <c r="B64" s="1">
+        <v>0.96</v>
+      </c>
       <c r="C64">
         <v>2404</v>
       </c>
@@ -1751,6 +1859,9 @@
       <c r="A66">
         <v>260</v>
       </c>
+      <c r="B66" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C66">
         <v>4452</v>
       </c>
@@ -1759,6 +1870,9 @@
       <c r="A67">
         <v>264</v>
       </c>
+      <c r="B67" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C67">
         <v>4452</v>
       </c>
@@ -1767,6 +1881,9 @@
       <c r="A68">
         <v>268</v>
       </c>
+      <c r="B68" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C68">
         <v>4452</v>
       </c>
@@ -1775,6 +1892,9 @@
       <c r="A69">
         <v>272</v>
       </c>
+      <c r="B69" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C69">
         <v>4452</v>
       </c>
@@ -1783,6 +1903,9 @@
       <c r="A70">
         <v>276</v>
       </c>
+      <c r="B70" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C70">
         <v>4452</v>
       </c>
@@ -1791,6 +1914,9 @@
       <c r="A71">
         <v>280</v>
       </c>
+      <c r="B71" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C71">
         <v>4452</v>
       </c>
@@ -1799,6 +1925,9 @@
       <c r="A72">
         <v>284</v>
       </c>
+      <c r="B72" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C72">
         <v>4452</v>
       </c>
@@ -1807,6 +1936,9 @@
       <c r="A73">
         <v>288</v>
       </c>
+      <c r="B73" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C73">
         <v>4452</v>
       </c>
@@ -1815,6 +1947,9 @@
       <c r="A74">
         <v>292</v>
       </c>
+      <c r="B74" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C74">
         <v>4452</v>
       </c>
@@ -1823,6 +1958,9 @@
       <c r="A75">
         <v>296</v>
       </c>
+      <c r="B75" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C75">
         <v>4452</v>
       </c>
@@ -1831,6 +1969,9 @@
       <c r="A76">
         <v>300</v>
       </c>
+      <c r="B76" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C76">
         <v>4452</v>
       </c>
@@ -1839,6 +1980,9 @@
       <c r="A77">
         <v>304</v>
       </c>
+      <c r="B77" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C77">
         <v>4452</v>
       </c>
@@ -1847,6 +1991,9 @@
       <c r="A78">
         <v>308</v>
       </c>
+      <c r="B78" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C78">
         <v>4452</v>
       </c>
@@ -1855,6 +2002,9 @@
       <c r="A79">
         <v>312</v>
       </c>
+      <c r="B79" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C79">
         <v>4452</v>
       </c>
@@ -1863,6 +2013,9 @@
       <c r="A80">
         <v>316</v>
       </c>
+      <c r="B80" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C80">
         <v>4452</v>
       </c>
@@ -1871,6 +2024,9 @@
       <c r="A81">
         <v>320</v>
       </c>
+      <c r="B81" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C81">
         <v>4452</v>
       </c>
@@ -1879,6 +2035,9 @@
       <c r="A82">
         <v>324</v>
       </c>
+      <c r="B82" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C82">
         <v>4452</v>
       </c>
@@ -1887,6 +2046,9 @@
       <c r="A83">
         <v>328</v>
       </c>
+      <c r="B83" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C83">
         <v>4452</v>
       </c>
@@ -1895,6 +2057,9 @@
       <c r="A84">
         <v>332</v>
       </c>
+      <c r="B84" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C84">
         <v>4452</v>
       </c>
@@ -1903,6 +2068,9 @@
       <c r="A85">
         <v>336</v>
       </c>
+      <c r="B85" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C85">
         <v>4452</v>
       </c>
@@ -1911,6 +2079,9 @@
       <c r="A86">
         <v>340</v>
       </c>
+      <c r="B86" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C86">
         <v>4452</v>
       </c>
@@ -1919,6 +2090,9 @@
       <c r="A87">
         <v>344</v>
       </c>
+      <c r="B87" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C87">
         <v>4452</v>
       </c>
@@ -1927,6 +2101,9 @@
       <c r="A88">
         <v>348</v>
       </c>
+      <c r="B88" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C88">
         <v>4452</v>
       </c>
@@ -1935,6 +2112,9 @@
       <c r="A89">
         <v>352</v>
       </c>
+      <c r="B89" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C89">
         <v>4452</v>
       </c>
@@ -1943,6 +2123,9 @@
       <c r="A90">
         <v>356</v>
       </c>
+      <c r="B90" s="1">
+        <v>0.98</v>
+      </c>
       <c r="C90">
         <v>4452</v>
       </c>
@@ -1951,6 +2134,9 @@
       <c r="A91">
         <v>360</v>
       </c>
+      <c r="B91" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C91">
         <v>4452</v>
       </c>
@@ -1959,6 +2145,9 @@
       <c r="A92">
         <v>364</v>
       </c>
+      <c r="B92" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C92">
         <v>4452</v>
       </c>
@@ -1967,6 +2156,9 @@
       <c r="A93">
         <v>368</v>
       </c>
+      <c r="B93" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C93">
         <v>4452</v>
       </c>
@@ -1975,6 +2167,9 @@
       <c r="A94">
         <v>372</v>
       </c>
+      <c r="B94" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C94">
         <v>4452</v>
       </c>
@@ -1983,6 +2178,9 @@
       <c r="A95">
         <v>376</v>
       </c>
+      <c r="B95" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C95">
         <v>4452</v>
       </c>
@@ -1991,6 +2189,9 @@
       <c r="A96">
         <v>380</v>
       </c>
+      <c r="B96" s="1">
+        <v>0.99</v>
+      </c>
       <c r="C96">
         <v>4452</v>
       </c>
@@ -1998,6 +2199,9 @@
     <row r="97" spans="1:3">
       <c r="A97">
         <v>384</v>
+      </c>
+      <c r="B97" s="1">
+        <v>0.99</v>
       </c>
       <c r="C97">
         <v>4452</v>
@@ -2025,7 +2229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78785FB9-A291-4E75-8EC1-3B24C941EE30}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
@@ -2122,7 +2326,7 @@
         <v>3630.0915300000001</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">(F3+G3)/D3</f>
+        <f t="shared" ref="I3:I9" si="0">(F3+G3)/D3</f>
         <v>4.4352585333006858E-2</v>
       </c>
     </row>
@@ -2341,5 +2545,6 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>